<commit_message>
[FIX] Muchos arreglos y avance en informe
</commit_message>
<xml_diff>
--- a/análisis/Requerimientos/No funcionales/RNF04 - Entrenamiento.xlsx
+++ b/análisis/Requerimientos/No funcionales/RNF04 - Entrenamiento.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -455,28 +455,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,7 +765,7 @@
   <dimension ref="B3:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:D12"/>
+      <selection activeCell="B5" sqref="B5:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,77 +792,77 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>